<commit_message>
fix specs and add 0.3.0 test for objective functions
</commit_message>
<xml_diff>
--- a/spec/files/discrete_dynamic_columns.xlsx
+++ b/spec/files/discrete_dynamic_columns.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19720" tabRatio="562" activeTab="2"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="14380" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="615">
   <si>
     <t># Variable</t>
   </si>
@@ -1867,6 +1867,12 @@
   </si>
   <si>
     <t>0.1.12</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>function group</t>
   </si>
 </sst>
 </file>
@@ -1926,7 +1932,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1981,6 +1987,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3462,7 +3474,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3531,6 +3543,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1469">
@@ -5724,7 +5743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
@@ -6064,9 +6083,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6092,36 +6111,42 @@
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" s="9" customFormat="1" ht="15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="33" t="s">
         <v>475</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="33" t="s">
         <v>477</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="33" t="s">
         <v>478</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="33" t="s">
         <v>479</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="33" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" s="15" customFormat="1" ht="15">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11" t="s">
+      <c r="G2" s="33" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="15" customFormat="1" ht="30">
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34" t="s">
         <v>480</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="34" t="s">
         <v>481</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="11"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="34" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">

</xml_diff>